<commit_message>
Mailing option for csa group activity notification
</commit_message>
<xml_diff>
--- a/scripts/Data/2019-results.xlsx
+++ b/scripts/Data/2019-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="mySheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,6 +34,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">姓名（</t>
     </r>
@@ -53,6 +54,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -64,6 +66,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">意向部门（</t>
     </r>
@@ -83,6 +86,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -94,6 +98,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">邮箱／</t>
     </r>
@@ -115,6 +120,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">微信号／</t>
     </r>
@@ -195,6 +201,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">部</t>
     </r>
@@ -223,6 +230,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">王亚珂 </t>
     </r>
@@ -296,6 +304,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">王志涵（</t>
     </r>
@@ -313,6 +322,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -367,17 +377,20 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -581,13 +594,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="86.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="6" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="12" min="6" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>